<commit_message>
actualizado ers | se agrega informe final calidad
</commit_message>
<xml_diff>
--- a/Fase 2/Evidencias Proyecto/documentacion/testing/3. Planilla Avance de Testing (semana 2).xlsx
+++ b/Fase 2/Evidencias Proyecto/documentacion/testing/3. Planilla Avance de Testing (semana 2).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\duoc\5to semestre\Portafolio\Portafolio_Grupo4_TatasApp\Fase 2\Evidencias Proyecto\documentacion\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6EFE423-5C8F-4C00-AB8D-2F474EAAFF5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E80C9F-3116-455A-A2FA-1ECB6EAA0A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="418">
   <si>
     <t>ID Test</t>
   </si>
@@ -1286,6 +1286,12 @@
   </si>
   <si>
     <t>P. BAJA</t>
+  </si>
+  <si>
+    <t>Total casos</t>
+  </si>
+  <si>
+    <t>%</t>
   </si>
 </sst>
 </file>
@@ -1392,20 +1398,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1488,7 +1481,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2504,7 +2497,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2541,6 +2534,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-DD60-4564-8C5C-28549B5178BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -2556,6 +2554,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-DD60-4564-8C5C-28549B5178BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -2571,6 +2574,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-DD60-4564-8C5C-28549B5178BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -2586,6 +2594,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-DD60-4564-8C5C-28549B5178BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -2692,6 +2705,315 @@
         </c:ser>
         <c:dLbls>
           <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>% de casos con error</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Métricas!$C$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-5440-4DAF-9AE9-B5DC69C8C321}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-5440-4DAF-9AE9-B5DC69C8C321}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-CL"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Métricas!$A$29:$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Con error</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sin error</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Métricas!$C$29:$C$30</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5440-4DAF-9AE9-B5DC69C8C321}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
@@ -2898,6 +3220,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
@@ -3921,6 +4283,525 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4544,6 +5425,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1547977-A9C5-A591-3261-EF2662B90257}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7540,8 +8457,8 @@
   </sheetPr>
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9737,10 +10654,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39AAE02B-5464-4B11-81BB-01D7F3AD180C}">
-  <dimension ref="A2:D25"/>
+  <dimension ref="A2:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -10006,6 +10923,57 @@
         <v>9</v>
       </c>
     </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="5">
+        <v>9</v>
+      </c>
+      <c r="C29" s="6">
+        <f>B29/$B$31</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="5">
+        <v>172</v>
+      </c>
+      <c r="C30" s="6">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="B31" s="5">
+        <v>180</v>
+      </c>
+      <c r="C31" s="6">
+        <f t="shared" ref="C30:C31" si="1">B31/$B$31</f>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>